<commit_message>
Intermediate changes for chechpoint 1
</commit_message>
<xml_diff>
--- a/Investments Case Study/Investments.xlsx
+++ b/Investments Case Study/Investments.xlsx
@@ -571,7 +571,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -671,6 +671,12 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1006,7 +1012,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1017,7 +1023,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1046,7 +1052,7 @@
       <c r="B3" s="25"/>
       <c r="C3" s="25"/>
     </row>
-    <row r="4" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
         <v>15</v>
       </c>
@@ -1057,25 +1063,25 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="5">
         <v>1</v>
       </c>
       <c r="B5" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="17">
+      <c r="C5" s="36">
         <v>66368</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5">
         <v>2</v>
       </c>
       <c r="B6" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="17">
+      <c r="C6" s="36">
         <v>66368</v>
       </c>
     </row>
@@ -1086,7 +1092,7 @@
       <c r="B7" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="17" t="s">
+      <c r="C7" s="37" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1097,7 +1103,7 @@
       <c r="B8" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="C8" s="17" t="s">
+      <c r="C8" s="36" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1108,9 +1114,9 @@
       <c r="B9" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="C9" s="17"/>
-    </row>
-    <row r="10" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="C9" s="36"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B10" s="11"/>
     </row>
     <row r="11" spans="1:3" ht="15" x14ac:dyDescent="0.25">
@@ -1132,6 +1138,7 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Checkins for Checkpoint 2 and 3
Code changes have been completed for checkpoint 2 and 3
</commit_message>
<xml_diff>
--- a/Investments Case Study/Investments.xlsx
+++ b/Investments Case Study/Investments.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7080"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7080" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Table -1.1" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="43">
   <si>
     <t>C1</t>
   </si>
@@ -355,6 +355,9 @@
   </si>
   <si>
     <t>N</t>
+  </si>
+  <si>
+    <t>Venture type is most suitable</t>
   </si>
 </sst>
 </file>
@@ -639,6 +642,12 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -671,12 +680,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1022,8 +1025,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1034,23 +1037,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="25"/>
+      <c r="B1" s="27"/>
       <c r="C1" s="15"/>
     </row>
     <row r="2" spans="1:3" ht="9.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="26"/>
-      <c r="B2" s="26"/>
+      <c r="A2" s="28"/>
+      <c r="B2" s="28"/>
       <c r="C2" s="15"/>
     </row>
     <row r="3" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
+      <c r="B3" s="27"/>
+      <c r="C3" s="27"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
@@ -1070,7 +1073,7 @@
       <c r="B5" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="36">
+      <c r="C5" s="25">
         <v>66368</v>
       </c>
     </row>
@@ -1081,7 +1084,7 @@
       <c r="B6" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="36">
+      <c r="C6" s="25">
         <v>66368</v>
       </c>
     </row>
@@ -1092,7 +1095,7 @@
       <c r="B7" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="37" t="s">
+      <c r="C7" s="26" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1103,7 +1106,7 @@
       <c r="B8" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="C8" s="36" t="s">
+      <c r="C8" s="25" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1114,7 +1117,9 @@
       <c r="B9" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="C9" s="36"/>
+      <c r="C9" s="25">
+        <v>114949</v>
+      </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B10" s="11"/>
@@ -1146,33 +1151,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="7.33203125" customWidth="1"/>
     <col min="2" max="2" width="53.88671875" customWidth="1"/>
-    <col min="3" max="3" width="23.88671875" customWidth="1"/>
+    <col min="3" max="3" width="25.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="27"/>
+      <c r="B1" s="29"/>
     </row>
     <row r="2" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="27"/>
-      <c r="B2" s="27"/>
+      <c r="A2" s="29"/>
+      <c r="B2" s="29"/>
     </row>
     <row r="3" spans="1:3" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="28" t="s">
+      <c r="A3" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="B3" s="28"/>
-      <c r="C3" s="28"/>
+      <c r="B3" s="30"/>
+      <c r="C3" s="30"/>
     </row>
     <row r="4" spans="1:3" s="2" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
@@ -1185,41 +1190,49 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="12">
         <v>1</v>
       </c>
       <c r="B5" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="12"/>
-    </row>
-    <row r="6" spans="1:3" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5" s="26">
+        <v>11748949</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="12">
         <v>2</v>
       </c>
       <c r="B6" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="12"/>
-    </row>
-    <row r="7" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="C6" s="26">
+        <v>958694.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="12">
         <v>3</v>
       </c>
       <c r="B7" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="12"/>
-    </row>
-    <row r="8" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="C7" s="26">
+        <v>719818</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="12">
         <v>4</v>
       </c>
       <c r="B8" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="12"/>
+      <c r="C8" s="26">
+        <v>73308593</v>
+      </c>
     </row>
     <row r="9" spans="1:3" ht="59.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="12">
@@ -1228,7 +1241,9 @@
       <c r="B9" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="C9" s="12"/>
+      <c r="C9" s="26" t="s">
+        <v>42</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1266,21 +1281,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="4" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="27"/>
+      <c r="B1" s="29"/>
     </row>
     <row r="2" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="29"/>
-      <c r="B2" s="29"/>
+      <c r="A2" s="31"/>
+      <c r="B2" s="31"/>
     </row>
     <row r="3" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="28" t="s">
+      <c r="A3" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="B3" s="28"/>
-      <c r="C3" s="28"/>
+      <c r="B3" s="30"/>
+      <c r="C3" s="30"/>
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
@@ -1357,23 +1372,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="31"/>
+      <c r="B1" s="33"/>
     </row>
     <row r="2" spans="1:5" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="32"/>
-      <c r="B2" s="33"/>
+      <c r="A2" s="34"/>
+      <c r="B2" s="35"/>
     </row>
     <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="34" t="s">
+      <c r="A3" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="B3" s="35"/>
-      <c r="C3" s="35"/>
-      <c r="D3" s="35"/>
-      <c r="E3" s="35"/>
+      <c r="B3" s="37"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
     </row>
     <row r="4" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="22" t="s">

</xml_diff>

<commit_message>
Changes for Checkpoint 5(partial checkin)
</commit_message>
<xml_diff>
--- a/Investments Case Study/Investments.xlsx
+++ b/Investments Case Study/Investments.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7080" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7080" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Table -1.1" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="49">
   <si>
     <t>C1</t>
   </si>
@@ -358,6 +358,24 @@
   </si>
   <si>
     <t>Venture type is most suitable</t>
+  </si>
+  <si>
+    <t>USA</t>
+  </si>
+  <si>
+    <t>Other Countries</t>
+  </si>
+  <si>
+    <t>GBR</t>
+  </si>
+  <si>
+    <t>Others</t>
+  </si>
+  <si>
+    <t>Cleantech &amp; Semiconductors</t>
+  </si>
+  <si>
+    <t>Social &amp; Finance &amp; Analytics &amp; Advertising</t>
   </si>
 </sst>
 </file>
@@ -1015,7 +1033,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1151,7 +1169,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
@@ -1270,7 +1288,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1315,7 +1333,9 @@
       <c r="B5" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="6"/>
+      <c r="C5" s="6" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="6" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
@@ -1324,7 +1344,9 @@
       <c r="B6" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="6"/>
+      <c r="C6" s="6" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="7" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
@@ -1333,7 +1355,9 @@
       <c r="B7" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="6"/>
+      <c r="C7" s="6" t="s">
+        <v>45</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1358,16 +1382,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8.88671875" style="1"/>
     <col min="2" max="2" width="56.88671875" customWidth="1"/>
-    <col min="3" max="3" width="17.44140625" customWidth="1"/>
-    <col min="4" max="4" width="14.88671875" customWidth="1"/>
+    <col min="3" max="3" width="35.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="3.109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1390,7 +1414,7 @@
       <c r="D3" s="37"/>
       <c r="E3" s="37"/>
     </row>
-    <row r="4" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="22" t="s">
         <v>3</v>
       </c>
@@ -1407,25 +1431,29 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="19">
         <v>1</v>
       </c>
       <c r="B5" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="17"/>
+      <c r="C5" s="17">
+        <v>12150</v>
+      </c>
       <c r="D5" s="17"/>
       <c r="E5" s="17"/>
     </row>
-    <row r="6" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="19">
         <v>2</v>
       </c>
       <c r="B6" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="17"/>
+      <c r="C6" s="17">
+        <v>108531347515</v>
+      </c>
       <c r="D6" s="17"/>
       <c r="E6" s="17"/>
     </row>
@@ -1436,7 +1464,9 @@
       <c r="B7" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="17"/>
+      <c r="C7" s="17" t="s">
+        <v>46</v>
+      </c>
       <c r="D7" s="17"/>
       <c r="E7" s="17"/>
     </row>
@@ -1447,7 +1477,9 @@
       <c r="B8" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="17"/>
+      <c r="C8" s="17" t="s">
+        <v>47</v>
+      </c>
       <c r="D8" s="17"/>
       <c r="E8" s="17"/>
     </row>
@@ -1458,7 +1490,9 @@
       <c r="B9" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="17"/>
+      <c r="C9" s="17" t="s">
+        <v>48</v>
+      </c>
       <c r="D9" s="17"/>
       <c r="E9" s="17"/>
     </row>
@@ -1469,7 +1503,9 @@
       <c r="B10" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="17"/>
+      <c r="C10" s="17">
+        <v>2923</v>
+      </c>
       <c r="D10" s="17"/>
       <c r="E10" s="17"/>
     </row>
@@ -1480,7 +1516,9 @@
       <c r="B11" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="17"/>
+      <c r="C11" s="17">
+        <v>2297</v>
+      </c>
       <c r="D11" s="17"/>
       <c r="E11" s="17"/>
     </row>
@@ -1491,7 +1529,9 @@
       <c r="B12" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="17"/>
+      <c r="C12" s="17">
+        <v>1912</v>
+      </c>
       <c r="D12" s="17"/>
       <c r="E12" s="17"/>
     </row>

</xml_diff>